<commit_message>
Remove original Status Summary section, update revenue chart to show revenue+expenses with totals, fix margin chart hover to show percentages
</commit_message>
<xml_diff>
--- a/public/Status Summary Source File.xlsx
+++ b/public/Status Summary Source File.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED111F0-CAF4-804C-8080-D7D8BB133163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EABD93-3047-2246-BE9A-F753ED3DEEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2240" windowWidth="28240" windowHeight="16020" xr2:uid="{E6CB5503-5085-A640-BB68-6722C76E813E}"/>
+    <workbookView xWindow="4440" yWindow="2240" windowWidth="25800" windowHeight="16020" xr2:uid="{E6CB5503-5085-A640-BB68-6722C76E813E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Total</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>July</t>
+  </si>
+  <si>
+    <t>Measures</t>
   </si>
 </sst>
 </file>
@@ -507,9 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FECB8AA-FBD7-9541-B5F0-05238F6D7C70}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -517,6 +518,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
@@ -571,7 +575,7 @@
         <v>933262.97000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -651,7 +655,7 @@
       </c>
       <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>-1.9442176226465928</v>
+        <v>-0.57888115061135248</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
@@ -714,7 +718,7 @@
         <v>117819.26000000001</v>
       </c>
       <c r="D7" s="2">
-        <v>231907.69000000003</v>
+        <v>124364</v>
       </c>
       <c r="E7" s="2">
         <v>96425.610000000015</v>

</xml_diff>

<commit_message>
Update Excel source files with new data
</commit_message>
<xml_diff>
--- a/public/Status Summary Source File.xlsx
+++ b/public/Status Summary Source File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-RMT-v2/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/expense_management_analytics-Wilmington/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EABD93-3047-2246-BE9A-F753ED3DEEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD18DF70-949D-DC4B-A3B7-C1A91618B602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2240" windowWidth="25800" windowHeight="16020" xr2:uid="{E6CB5503-5085-A640-BB68-6722C76E813E}"/>
+    <workbookView xWindow="2920" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{E6CB5503-5085-A640-BB68-6722C76E813E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Total</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Jun</t>
-  </si>
-  <si>
-    <t>July</t>
   </si>
   <si>
     <t>Measures</t>
@@ -508,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FECB8AA-FBD7-9541-B5F0-05238F6D7C70}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -517,9 +514,9 @@
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>7</v>
@@ -540,200 +537,181 @@
         <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>141764.06999999998</v>
+        <v>124559.84</v>
       </c>
       <c r="C2" s="2">
-        <v>115152.98</v>
+        <v>116465.91</v>
       </c>
       <c r="D2" s="2">
-        <v>144090.18</v>
+        <v>102788.45</v>
       </c>
       <c r="E2" s="2">
-        <v>147081.04</v>
+        <v>124082.6</v>
       </c>
       <c r="F2" s="2">
-        <v>81394.06</v>
+        <v>101734.84</v>
       </c>
       <c r="G2" s="2">
-        <v>138129</v>
+        <v>104787.57</v>
       </c>
       <c r="H2" s="2">
-        <v>165651.64000000001</v>
-      </c>
-      <c r="I2" s="2">
-        <v>933262.97000000009</v>
+        <f>SUM(B2:G2)</f>
+        <v>674419.21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>129293.65999999997</v>
+        <v>122998.31</v>
       </c>
       <c r="C3" s="2">
-        <v>105455.49999999999</v>
+        <v>127047.08</v>
       </c>
       <c r="D3" s="2">
-        <v>114676.70999999999</v>
+        <v>124268.94</v>
       </c>
       <c r="E3" s="2">
-        <v>94162.760000000038</v>
+        <v>131430.51999999999</v>
       </c>
       <c r="F3" s="2">
-        <v>129991.53000000001</v>
+        <v>156847.54999999999</v>
       </c>
       <c r="G3" s="2">
-        <v>108666.03999999998</v>
+        <v>116550.34</v>
       </c>
       <c r="H3" s="2">
-        <v>106077.50000000003</v>
-      </c>
-      <c r="I3" s="2">
-        <v>788323.7</v>
+        <f>SUM(B3:G3)</f>
+        <v>779142.73999999987</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4">
         <f>(B2-B3)/B2</f>
-        <v>8.7965942287068971E-2</v>
+        <v>1.2536384118669379E-2</v>
       </c>
       <c r="C4" s="4">
-        <f t="shared" ref="C4:I4" si="0">(C2-C3)/C2</f>
-        <v>8.421388660545312E-2</v>
+        <f t="shared" ref="C4:H4" si="0">(C2-C3)/C2</f>
+        <v>-9.0852078518083079E-2</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
-        <v>0.20413237043634758</v>
+        <v>-0.20897766237354495</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>0.35978994981270168</v>
+        <v>-5.9217972544095492E-2</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
-        <v>-0.59706408551189138</v>
+        <v>-0.54172896915157087</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>0.21330032071469437</v>
+        <v>-0.11225348579034697</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" si="0"/>
-        <v>0.35963507514927096</v>
-      </c>
-      <c r="I4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.15530378324128741</v>
+        <v>-0.15527957751974461</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4">
         <f>(B6-B7)/B6</f>
-        <v>4.9754171205877142E-2</v>
+        <v>-0.32757369391969843</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:I5" si="1">(C6-C7)/C6</f>
-        <v>-0.10156148396279288</v>
+        <f t="shared" ref="C5:H5" si="1">(C6-C7)/C6</f>
+        <v>-0.40761108752331504</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>-0.57888115061135248</v>
+        <v>-0.50264118422665316</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>-8.274341922425886E-2</v>
+        <v>-1.0622256961751353</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="1"/>
-        <v>-0.11303279806102753</v>
+        <v>-0.75601424823928087</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="1"/>
-        <v>-6.8571683765040782E-3</v>
+        <v>-0.68984407856353691</v>
       </c>
       <c r="H5" s="4">
         <f t="shared" si="1"/>
-        <v>-0.42852614327765792</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="1"/>
-        <v>-0.30117364158099841</v>
+        <v>-0.60676257265368638</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>146886.78</v>
+        <v>89259.06</v>
       </c>
       <c r="C6" s="2">
-        <v>106956.59</v>
+        <v>77299.86</v>
       </c>
       <c r="D6" s="2">
-        <v>78767.17</v>
+        <v>72777.960000000006</v>
       </c>
       <c r="E6" s="2">
-        <v>89056.75</v>
+        <v>66949.03</v>
       </c>
       <c r="F6" s="2">
-        <v>106934.98</v>
+        <v>77545.02</v>
       </c>
       <c r="G6" s="2">
-        <v>88672.17</v>
+        <v>70120.570000000007</v>
       </c>
       <c r="H6" s="2">
-        <v>71830.319999999992</v>
-      </c>
-      <c r="I6" s="2">
-        <v>689104.76</v>
+        <f>SUM(B6:G6)</f>
+        <v>453951.50000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>139578.54999999999</v>
+        <v>118497.98</v>
       </c>
       <c r="C7" s="2">
-        <v>117819.26000000001</v>
+        <v>108808.14</v>
       </c>
       <c r="D7" s="2">
-        <v>124364</v>
+        <v>109359.16</v>
       </c>
       <c r="E7" s="2">
-        <v>96425.610000000015</v>
+        <v>138064.01</v>
       </c>
       <c r="F7" s="2">
-        <v>119022.14000000001</v>
+        <v>136170.16</v>
       </c>
       <c r="G7" s="2">
-        <v>89280.209999999992</v>
+        <v>118492.83</v>
       </c>
       <c r="H7" s="2">
-        <v>102611.49</v>
-      </c>
-      <c r="I7" s="2">
-        <v>896644.95</v>
+        <f>SUM(B7:G7)</f>
+        <v>729392.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>